<commit_message>
Update Usability sheet file.
</commit_message>
<xml_diff>
--- a/files/templates/Usability_Report.xlsx
+++ b/files/templates/Usability_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vidp\erp\printerp\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07975909-7E0F-440F-B46E-253A4F0B019F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47EAF8C-9485-430B-A439-618C3B846900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Q$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>No</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Machine</t>
+  </si>
+  <si>
+    <t>Internal Use</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
   </si>
 </sst>
 </file>
@@ -119,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,58 +424,60 @@
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H1" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
@@ -475,23 +486,29 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Q2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
-    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Usability 2022-11-25 16:04
</commit_message>
<xml_diff>
--- a/files/templates/Usability_Report.xlsx
+++ b/files/templates/Usability_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vidp\erp\printerp\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47EAF8C-9485-430B-A439-618C3B846900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7668CC9E-ED9E-47AB-B195-C0D63E68FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
Update Usability sheet template
</commit_message>
<xml_diff>
--- a/files/templates/Usability_Report.xlsx
+++ b/files/templates/Usability_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vidp\erp\printerp\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7668CC9E-ED9E-47AB-B195-C0D63E68FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FC5F5F-D76C-4F72-A26E-285C454D97F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Q$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$S$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -125,8 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,9 +425,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -427,31 +441,31 @@
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="6" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J1" s="3" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
+      <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,23 +481,23 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
@@ -492,23 +506,29 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Q2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:S2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>